<commit_message>
writing draft in progress
</commit_message>
<xml_diff>
--- a/data/2020 Beach Sampling Compiled Results_FINALREPORT.xlsx
+++ b/data/2020 Beach Sampling Compiled Results_FINALREPORT.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bmeyer\Documents\KWF_Beach_Sampling_2019_2020\KWF_Beach_Sampling_2019_2020\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bmeyer\Documents\GitHub\KWF_Beach_Sampling_2019_2020\KWF_Beach_Sampling_2019_2020\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="803" firstSheet="5" activeTab="6"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="803" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="2020 READ THIS FIRST" sheetId="28" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="221">
   <si>
     <t>Sample Date</t>
   </si>
@@ -1116,6 +1116,9 @@
   </si>
   <si>
     <t>Aug 28</t>
+  </si>
+  <si>
+    <t>Look up full def here; do they mean no more thn 10% of sampes from season, or for 30 days?  If its for 30 days, there should be2-3 values per column at each site</t>
   </si>
 </sst>
 </file>
@@ -3997,12 +4000,9 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>[1]Sheet1!$B$1</c:f>
+              <c:f>[1]Sheet1!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>2020</c:v>
-                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
@@ -4020,359 +4020,44 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>[1]Sheet1!$A$2:$A$60</c:f>
+              <c:f>[1]Sheet1!$A$2:$A$65</c:f>
               <c:strCache>
-                <c:ptCount val="59"/>
-                <c:pt idx="0">
-                  <c:v>July 1</c:v>
-                </c:pt>
+                <c:ptCount val="64"/>
                 <c:pt idx="1">
-                  <c:v>July 2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>July 3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>July 4</c:v>
+                  <c:v>B (Water Recreation)  Fail / Pass</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>July 5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>July 6</c:v>
+                  <c:v>Warren Ames Bridge</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>July 7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>July 8</c:v>
+                  <c:v>Kenai River Gull Rookery 1</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>July 9</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>July 10</c:v>
+                  <c:v>Kenai River Gull Rookery 2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>July 11</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>July 12</c:v>
+                  <c:v>South Kenai Beach 3</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>July 13</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>July 14</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>July 15</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>July 16</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>July 17</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>July 18</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>July 19</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>July 20</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>July 21</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>July 22</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>July 23</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>July 24</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>July 25</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>July 26</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>July 27</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>July 28</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>July 29</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>July 30</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>July 31</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>Aug 1</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>Aug 2</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>Aug 3</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>Aug 4</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>Aug 5</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>Aug 6</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>Aug 7</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>Aug 8</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>Aug 9</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>Aug 10</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>Aug 11</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>Aug 12</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>Aug 13</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>Aug 14</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>Aug 15</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>Aug 16</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>Aug 17</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>Aug 18</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>Aug 19</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>Aug 20</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>Aug 21</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>Aug 22</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>Aug 23</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>Aug 24</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>Aug 25</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>Aug 26</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>Aug 27</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>Aug 28</c:v>
+                  <c:v>North Kenai Beach 4</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>[1]Sheet1!$B$2:$B$60</c:f>
+              <c:f>[1]Sheet1!$C$2:$C$65</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="59"/>
-                <c:pt idx="0">
-                  <c:v>5355</c:v>
-                </c:pt>
+                <c:ptCount val="64"/>
                 <c:pt idx="1">
-                  <c:v>3468</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3576</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3965</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4290</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>11190</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>15138</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>12127</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>8686</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>6032</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>10104</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>16526</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>36247</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>30084</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>34662</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>19086</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>31392</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>26143</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>32598</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>46306</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>17854</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>17316</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>20172</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>20562</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>23922</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>20117</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>38004</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>47946</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>40632</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>43048</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>40718</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>24792</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>37548</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>43706</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>41152</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>39293</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>40686</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>26737</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>25520</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>35474</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>24791</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>44123</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>49097</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>65900</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>107241</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>70055</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>112174</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>134874</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>56939</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>15709</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>43468</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>43826</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>20828</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>17402</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>4785</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4389,12 +4074,9 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>[1]Sheet1!$C$1</c:f>
+              <c:f>[1]Sheet1!$E$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>2019</c:v>
-                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
@@ -4412,344 +4094,41 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>[1]Sheet1!$A$2:$A$60</c:f>
+              <c:f>[1]Sheet1!$A$2:$A$65</c:f>
               <c:strCache>
-                <c:ptCount val="59"/>
-                <c:pt idx="0">
-                  <c:v>July 1</c:v>
-                </c:pt>
+                <c:ptCount val="64"/>
                 <c:pt idx="1">
-                  <c:v>July 2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>July 3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>July 4</c:v>
+                  <c:v>B (Water Recreation)  Fail / Pass</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>July 5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>July 6</c:v>
+                  <c:v>Warren Ames Bridge</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>July 7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>July 8</c:v>
+                  <c:v>Kenai River Gull Rookery 1</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>July 9</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>July 10</c:v>
+                  <c:v>Kenai River Gull Rookery 2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>July 11</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>July 12</c:v>
+                  <c:v>South Kenai Beach 3</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>July 13</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>July 14</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>July 15</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>July 16</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>July 17</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>July 18</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>July 19</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>July 20</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>July 21</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>July 22</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>July 23</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>July 24</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>July 25</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>July 26</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>July 27</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>July 28</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>July 29</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>July 30</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>July 31</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>Aug 1</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>Aug 2</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>Aug 3</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>Aug 4</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>Aug 5</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>Aug 6</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>Aug 7</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>Aug 8</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>Aug 9</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>Aug 10</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>Aug 11</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>Aug 12</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>Aug 13</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>Aug 14</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>Aug 15</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>Aug 16</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>Aug 17</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>Aug 18</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>Aug 19</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>Aug 20</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>Aug 21</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>Aug 22</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>Aug 23</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>Aug 24</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>Aug 25</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>Aug 26</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>Aug 27</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>Aug 28</c:v>
+                  <c:v>North Kenai Beach 4</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>[1]Sheet1!$C$2:$C$60</c:f>
+              <c:f>[1]Sheet1!$E$2:$E$65</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="59"/>
-                <c:pt idx="0">
-                  <c:v>6810</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>7230</c:v>
-                </c:pt>
+                <c:ptCount val="64"/>
                 <c:pt idx="2">
-                  <c:v>6250</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7740</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>8472</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>9093</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>12621</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>21444</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>15190</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10485</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>14098</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>22868</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>20130</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>34054</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>30509</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>16420</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>23285</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>46059</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>25963</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>35652</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>76650</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>75542</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>36107</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>53574</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>80928</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>77996</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>98201</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>99038</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>75604</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>42439</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>34315</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>37711</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>42084</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>55930</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>62687</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>72712</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>76394</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>61264</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>48046</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>37042</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>32759</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>32146</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>25377</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>22158</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>25809</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>24908</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>22220</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>18146</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>16763</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>10131</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4766,12 +4145,9 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>[1]Sheet1!$D$1</c:f>
+              <c:f>[1]Sheet1!$H$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>2018</c:v>
-                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
@@ -4789,371 +4165,74 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>[1]Sheet1!$A$2:$A$60</c:f>
+              <c:f>[1]Sheet1!$A$2:$A$65</c:f>
               <c:strCache>
-                <c:ptCount val="59"/>
-                <c:pt idx="0">
-                  <c:v>July 1</c:v>
-                </c:pt>
+                <c:ptCount val="64"/>
                 <c:pt idx="1">
-                  <c:v>July 2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>July 3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>July 4</c:v>
+                  <c:v>B (Water Recreation)  Fail / Pass</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>July 5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>July 6</c:v>
+                  <c:v>Warren Ames Bridge</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>July 7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>July 8</c:v>
+                  <c:v>Kenai River Gull Rookery 1</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>July 9</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>July 10</c:v>
+                  <c:v>Kenai River Gull Rookery 2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>July 11</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>July 12</c:v>
+                  <c:v>South Kenai Beach 3</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>July 13</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>July 14</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>July 15</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>July 16</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>July 17</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>July 18</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>July 19</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>July 20</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>July 21</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>July 22</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>July 23</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>July 24</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>July 25</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>July 26</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>July 27</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>July 28</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>July 29</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>July 30</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>July 31</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>Aug 1</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>Aug 2</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>Aug 3</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>Aug 4</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>Aug 5</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>Aug 6</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>Aug 7</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>Aug 8</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>Aug 9</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>Aug 10</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>Aug 11</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>Aug 12</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>Aug 13</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>Aug 14</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>Aug 15</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>Aug 16</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>Aug 17</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>Aug 18</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>Aug 19</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>Aug 20</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>Aug 21</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>Aug 22</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>Aug 23</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>Aug 24</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>Aug 25</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>Aug 26</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>Aug 27</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>Aug 28</c:v>
+                  <c:v>North Kenai Beach 4</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>[1]Sheet1!$D$2:$D$60</c:f>
+              <c:f>[1]Sheet1!$H$2:$H$65</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="59"/>
-                <c:pt idx="0">
-                  <c:v>1966</c:v>
-                </c:pt>
+                <c:ptCount val="64"/>
                 <c:pt idx="1">
-                  <c:v>3694</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2394</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4559</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5065</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6505</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7786</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5544</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5724</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3744</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4062</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>14898</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>23394</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>8593</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>7662</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>7110</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>11072</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>19280</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>30293</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>33858</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>62503</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>24618</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>33606</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>25466</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>14129</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>15316</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>16043</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>8923</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>11482</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>14879</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>18579</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>22734</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>17967</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>22848</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>27423</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>31944</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>30190</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>55768</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>11146</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>14372</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>14265</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>26837</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>40040</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>16205</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>6692</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>12195</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>18030</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>23000</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>26642</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>29068</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>27787</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>17005</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>6539</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>28895</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>17189</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>19651</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>7795</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>9351</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>1436</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5170,12 +4249,9 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>[1]Sheet1!$E$1</c:f>
+              <c:f>[1]Sheet1!$I$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>2017</c:v>
-                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
@@ -5193,359 +4269,38 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>[1]Sheet1!$A$2:$A$60</c:f>
+              <c:f>[1]Sheet1!$A$2:$A$65</c:f>
               <c:strCache>
-                <c:ptCount val="59"/>
-                <c:pt idx="0">
-                  <c:v>July 1</c:v>
-                </c:pt>
+                <c:ptCount val="64"/>
                 <c:pt idx="1">
-                  <c:v>July 2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>July 3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>July 4</c:v>
+                  <c:v>B (Water Recreation)  Fail / Pass</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>July 5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>July 6</c:v>
+                  <c:v>Warren Ames Bridge</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>July 7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>July 8</c:v>
+                  <c:v>Kenai River Gull Rookery 1</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>July 9</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>July 10</c:v>
+                  <c:v>Kenai River Gull Rookery 2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>July 11</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>July 12</c:v>
+                  <c:v>South Kenai Beach 3</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>July 13</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>July 14</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>July 15</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>July 16</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>July 17</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>July 18</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>July 19</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>July 20</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>July 21</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>July 22</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>July 23</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>July 24</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>July 25</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>July 26</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>July 27</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>July 28</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>July 29</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>July 30</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>July 31</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>Aug 1</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>Aug 2</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>Aug 3</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>Aug 4</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>Aug 5</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>Aug 6</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>Aug 7</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>Aug 8</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>Aug 9</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>Aug 10</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>Aug 11</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>Aug 12</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>Aug 13</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>Aug 14</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>Aug 15</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>Aug 16</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>Aug 17</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>Aug 18</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>Aug 19</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>Aug 20</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>Aug 21</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>Aug 22</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>Aug 23</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>Aug 24</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>Aug 25</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>Aug 26</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>Aug 27</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>Aug 28</c:v>
+                  <c:v>North Kenai Beach 4</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>[1]Sheet1!$E$2:$E$60</c:f>
+              <c:f>[1]Sheet1!$I$2:$I$65</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="59"/>
-                <c:pt idx="0">
-                  <c:v>2924</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4088</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4880</c:v>
-                </c:pt>
+                <c:ptCount val="64"/>
                 <c:pt idx="3">
-                  <c:v>8652</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>8833</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5676</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>9688</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>12138</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>17946</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>19932</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>9390</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>11330</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>8346</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>6565</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>9180</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>10185</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>30081</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>30486</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>24480</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>29730</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>27450</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>14280</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>27864</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>48467</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>59951</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>71904</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>66624</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>53887</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>56765</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>25104</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>30523</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>30222</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>13064</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>23180</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>20405</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>17137</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>32544</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>56283</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>30678</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>13072</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>8620</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>13168</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>18558</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>30833</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>35256</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>21046</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>16629</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>30362</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>33151</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>32187</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>23203</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>20586</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>12087</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>12268</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>16610</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6476,976 +5231,153 @@
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Sheet1"/>
+      <sheetName val="Sheet2"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
-        <row r="1">
-          <cell r="B1">
-            <v>2020</v>
-          </cell>
-          <cell r="C1">
-            <v>2019</v>
-          </cell>
-          <cell r="D1">
-            <v>2018</v>
-          </cell>
-          <cell r="E1">
-            <v>2017</v>
-          </cell>
-        </row>
-        <row r="2">
-          <cell r="A2" t="str">
-            <v>July 1</v>
-          </cell>
-          <cell r="B2">
-            <v>5355</v>
-          </cell>
-          <cell r="C2">
-            <v>6810</v>
-          </cell>
-          <cell r="D2">
-            <v>1966</v>
-          </cell>
-          <cell r="E2">
-            <v>2924</v>
-          </cell>
-        </row>
         <row r="3">
           <cell r="A3" t="str">
-            <v>July 2</v>
+            <v>B (Water Recreation)  Fail / Pass</v>
           </cell>
-          <cell r="B3">
-            <v>3468</v>
+          <cell r="C3" t="str">
+            <v>Fecal Coliform</v>
           </cell>
-          <cell r="C3">
-            <v>7230</v>
+          <cell r="E3"/>
+          <cell r="H3" t="str">
+            <v>Enterococci</v>
           </cell>
-          <cell r="D3">
-            <v>3694</v>
-          </cell>
-          <cell r="E3">
-            <v>4088</v>
-          </cell>
+          <cell r="I3"/>
         </row>
         <row r="4">
-          <cell r="A4" t="str">
-            <v>July 3</v>
+          <cell r="A4"/>
+          <cell r="C4" t="str">
+            <v>Secondary recreation</v>
           </cell>
-          <cell r="B4">
-            <v>3576</v>
+          <cell r="E4" t="str">
+            <v>Harvesting for consumption of raw mollusks or other raw aquatic life</v>
           </cell>
-          <cell r="C4">
-            <v>6250</v>
+          <cell r="H4" t="str">
+            <v>Contact recreation</v>
           </cell>
-          <cell r="D4">
-            <v>2394</v>
-          </cell>
-          <cell r="E4">
-            <v>4880</v>
-          </cell>
+          <cell r="I4"/>
         </row>
         <row r="5">
-          <cell r="A5" t="str">
-            <v>July 4</v>
+          <cell r="A5"/>
+          <cell r="C5" t="str">
+            <v>30-day geometric mean of samples may not exceed 200 CFU/100 mL</v>
           </cell>
-          <cell r="B5">
-            <v>3965</v>
+          <cell r="E5" t="str">
+            <v>30-day geometric mean of samples may not exceed 14 CFU/100 mL</v>
           </cell>
-          <cell r="C5">
-            <v>7740</v>
+          <cell r="H5" t="str">
+            <v>In a 30-day period, not more than 10% of individual samples may exceed 130 CFU/100 mL</v>
           </cell>
-          <cell r="D5">
-            <v>4559</v>
-          </cell>
-          <cell r="E5">
-            <v>8652</v>
+          <cell r="I5" t="str">
+            <v>30-day geometric mean of samples may not exceed 35 CFU/100 mL</v>
           </cell>
         </row>
         <row r="6">
           <cell r="A6" t="str">
-            <v>July 5</v>
+            <v>Warren Ames Bridge</v>
           </cell>
-          <cell r="B6">
-            <v>4290</v>
+          <cell r="C6"/>
+          <cell r="E6"/>
+          <cell r="H6" t="str">
+            <v>0/4</v>
           </cell>
-          <cell r="C6">
-            <v>8472</v>
-          </cell>
-          <cell r="D6">
-            <v>5065</v>
-          </cell>
-          <cell r="E6">
-            <v>8833</v>
-          </cell>
+          <cell r="I6"/>
         </row>
         <row r="7">
-          <cell r="A7" t="str">
-            <v>July 6</v>
+          <cell r="A7"/>
+          <cell r="C7"/>
+          <cell r="E7"/>
+          <cell r="H7" t="str">
+            <v>0/4</v>
           </cell>
-          <cell r="B7">
-            <v>11190</v>
-          </cell>
-          <cell r="C7">
-            <v>9093</v>
-          </cell>
-          <cell r="D7">
-            <v>6505</v>
-          </cell>
-          <cell r="E7">
-            <v>5676</v>
-          </cell>
+          <cell r="I7"/>
         </row>
         <row r="8">
           <cell r="A8" t="str">
-            <v>July 7</v>
+            <v>Kenai River Gull Rookery 1</v>
           </cell>
-          <cell r="B8">
-            <v>15138</v>
+          <cell r="C8"/>
+          <cell r="E8"/>
+          <cell r="H8" t="str">
+            <v>0/4</v>
           </cell>
-          <cell r="C8">
-            <v>12621</v>
-          </cell>
-          <cell r="D8">
-            <v>7786</v>
-          </cell>
-          <cell r="E8">
-            <v>9688</v>
-          </cell>
+          <cell r="I8"/>
         </row>
         <row r="9">
-          <cell r="A9" t="str">
-            <v>July 8</v>
+          <cell r="A9"/>
+          <cell r="C9"/>
+          <cell r="E9"/>
+          <cell r="H9" t="str">
+            <v>0/4</v>
           </cell>
-          <cell r="B9">
-            <v>12127</v>
-          </cell>
-          <cell r="C9">
-            <v>21444</v>
-          </cell>
-          <cell r="D9">
-            <v>5544</v>
-          </cell>
-          <cell r="E9">
-            <v>12138</v>
-          </cell>
+          <cell r="I9"/>
         </row>
         <row r="10">
           <cell r="A10" t="str">
-            <v>July 9</v>
+            <v>Kenai River Gull Rookery 2</v>
           </cell>
-          <cell r="B10">
-            <v>8686</v>
+          <cell r="C10"/>
+          <cell r="E10"/>
+          <cell r="H10" t="str">
+            <v>0/4</v>
           </cell>
-          <cell r="C10">
-            <v>15190</v>
-          </cell>
-          <cell r="D10">
-            <v>5724</v>
-          </cell>
-          <cell r="E10">
-            <v>17946</v>
-          </cell>
+          <cell r="I10"/>
         </row>
         <row r="11">
-          <cell r="A11" t="str">
-            <v>July 10</v>
+          <cell r="A11"/>
+          <cell r="C11"/>
+          <cell r="E11"/>
+          <cell r="H11" t="str">
+            <v>0/4</v>
           </cell>
-          <cell r="B11">
-            <v>6032</v>
-          </cell>
-          <cell r="C11">
-            <v>10485</v>
-          </cell>
-          <cell r="D11">
-            <v>3744</v>
-          </cell>
-          <cell r="E11">
-            <v>19932</v>
-          </cell>
+          <cell r="I11"/>
         </row>
         <row r="12">
           <cell r="A12" t="str">
-            <v>July 11</v>
+            <v>South Kenai Beach 3</v>
           </cell>
-          <cell r="B12">
-            <v>10104</v>
+          <cell r="C12"/>
+          <cell r="E12"/>
+          <cell r="H12" t="str">
+            <v>2/5</v>
           </cell>
-          <cell r="C12">
-            <v>14098</v>
-          </cell>
-          <cell r="D12">
-            <v>4062</v>
-          </cell>
-          <cell r="E12">
-            <v>9390</v>
-          </cell>
+          <cell r="I12"/>
         </row>
         <row r="13">
-          <cell r="A13" t="str">
-            <v>July 12</v>
+          <cell r="A13"/>
+          <cell r="C13"/>
+          <cell r="E13"/>
+          <cell r="H13" t="str">
+            <v>0/5</v>
           </cell>
-          <cell r="B13">
-            <v>16526</v>
-          </cell>
-          <cell r="C13">
-            <v>22868</v>
-          </cell>
-          <cell r="D13">
-            <v>14898</v>
-          </cell>
-          <cell r="E13">
-            <v>11330</v>
-          </cell>
+          <cell r="I13"/>
         </row>
         <row r="14">
           <cell r="A14" t="str">
-            <v>July 13</v>
+            <v>North Kenai Beach 4</v>
           </cell>
-          <cell r="B14">
-            <v>36247</v>
+          <cell r="C14"/>
+          <cell r="E14"/>
+          <cell r="H14" t="str">
+            <v>0/5</v>
           </cell>
-          <cell r="C14">
-            <v>20130</v>
-          </cell>
-          <cell r="D14">
-            <v>23394</v>
-          </cell>
-          <cell r="E14">
-            <v>8346</v>
-          </cell>
+          <cell r="I14"/>
         </row>
         <row r="15">
-          <cell r="A15" t="str">
-            <v>July 14</v>
+          <cell r="A15"/>
+          <cell r="C15"/>
+          <cell r="E15"/>
+          <cell r="H15" t="str">
+            <v>0/5</v>
           </cell>
-          <cell r="B15">
-            <v>30084</v>
-          </cell>
-          <cell r="C15">
-            <v>34054</v>
-          </cell>
-          <cell r="D15">
-            <v>8593</v>
-          </cell>
-          <cell r="E15">
-            <v>6565</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="A16" t="str">
-            <v>July 15</v>
-          </cell>
-          <cell r="B16">
-            <v>34662</v>
-          </cell>
-          <cell r="C16">
-            <v>30509</v>
-          </cell>
-          <cell r="D16">
-            <v>7662</v>
-          </cell>
-          <cell r="E16">
-            <v>9180</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="A17" t="str">
-            <v>July 16</v>
-          </cell>
-          <cell r="B17">
-            <v>19086</v>
-          </cell>
-          <cell r="C17">
-            <v>16420</v>
-          </cell>
-          <cell r="D17">
-            <v>7110</v>
-          </cell>
-          <cell r="E17">
-            <v>10185</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="A18" t="str">
-            <v>July 17</v>
-          </cell>
-          <cell r="B18">
-            <v>31392</v>
-          </cell>
-          <cell r="C18">
-            <v>23285</v>
-          </cell>
-          <cell r="D18">
-            <v>11072</v>
-          </cell>
-          <cell r="E18">
-            <v>30081</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="A19" t="str">
-            <v>July 18</v>
-          </cell>
-          <cell r="B19">
-            <v>26143</v>
-          </cell>
-          <cell r="C19">
-            <v>46059</v>
-          </cell>
-          <cell r="D19">
-            <v>19280</v>
-          </cell>
-          <cell r="E19">
-            <v>30486</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="A20" t="str">
-            <v>July 19</v>
-          </cell>
-          <cell r="B20">
-            <v>32598</v>
-          </cell>
-          <cell r="C20">
-            <v>25963</v>
-          </cell>
-          <cell r="D20">
-            <v>30293</v>
-          </cell>
-          <cell r="E20">
-            <v>24480</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="A21" t="str">
-            <v>July 20</v>
-          </cell>
-          <cell r="B21">
-            <v>46306</v>
-          </cell>
-          <cell r="C21">
-            <v>35652</v>
-          </cell>
-          <cell r="D21">
-            <v>33858</v>
-          </cell>
-          <cell r="E21">
-            <v>29730</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="A22" t="str">
-            <v>July 21</v>
-          </cell>
-          <cell r="B22">
-            <v>17854</v>
-          </cell>
-          <cell r="C22">
-            <v>76650</v>
-          </cell>
-          <cell r="D22">
-            <v>62503</v>
-          </cell>
-          <cell r="E22">
-            <v>27450</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="A23" t="str">
-            <v>July 22</v>
-          </cell>
-          <cell r="B23">
-            <v>17316</v>
-          </cell>
-          <cell r="C23">
-            <v>75542</v>
-          </cell>
-          <cell r="D23">
-            <v>24618</v>
-          </cell>
-          <cell r="E23">
-            <v>14280</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="A24" t="str">
-            <v>July 23</v>
-          </cell>
-          <cell r="B24">
-            <v>20172</v>
-          </cell>
-          <cell r="C24">
-            <v>36107</v>
-          </cell>
-          <cell r="D24">
-            <v>33606</v>
-          </cell>
-          <cell r="E24">
-            <v>27864</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="A25" t="str">
-            <v>July 24</v>
-          </cell>
-          <cell r="B25">
-            <v>20562</v>
-          </cell>
-          <cell r="C25">
-            <v>53574</v>
-          </cell>
-          <cell r="D25">
-            <v>25466</v>
-          </cell>
-          <cell r="E25">
-            <v>48467</v>
-          </cell>
-        </row>
-        <row r="26">
-          <cell r="A26" t="str">
-            <v>July 25</v>
-          </cell>
-          <cell r="B26">
-            <v>23922</v>
-          </cell>
-          <cell r="C26">
-            <v>80928</v>
-          </cell>
-          <cell r="D26">
-            <v>14129</v>
-          </cell>
-          <cell r="E26">
-            <v>59951</v>
-          </cell>
-        </row>
-        <row r="27">
-          <cell r="A27" t="str">
-            <v>July 26</v>
-          </cell>
-          <cell r="B27">
-            <v>20117</v>
-          </cell>
-          <cell r="C27">
-            <v>77996</v>
-          </cell>
-          <cell r="D27">
-            <v>15316</v>
-          </cell>
-          <cell r="E27">
-            <v>71904</v>
-          </cell>
-        </row>
-        <row r="28">
-          <cell r="A28" t="str">
-            <v>July 27</v>
-          </cell>
-          <cell r="B28">
-            <v>38004</v>
-          </cell>
-          <cell r="C28">
-            <v>98201</v>
-          </cell>
-          <cell r="D28">
-            <v>16043</v>
-          </cell>
-          <cell r="E28">
-            <v>66624</v>
-          </cell>
-        </row>
-        <row r="29">
-          <cell r="A29" t="str">
-            <v>July 28</v>
-          </cell>
-          <cell r="B29">
-            <v>47946</v>
-          </cell>
-          <cell r="C29">
-            <v>99038</v>
-          </cell>
-          <cell r="D29">
-            <v>8923</v>
-          </cell>
-          <cell r="E29">
-            <v>53887</v>
-          </cell>
-        </row>
-        <row r="30">
-          <cell r="A30" t="str">
-            <v>July 29</v>
-          </cell>
-          <cell r="B30">
-            <v>40632</v>
-          </cell>
-          <cell r="C30">
-            <v>75604</v>
-          </cell>
-          <cell r="D30">
-            <v>11482</v>
-          </cell>
-          <cell r="E30">
-            <v>56765</v>
-          </cell>
-        </row>
-        <row r="31">
-          <cell r="A31" t="str">
-            <v>July 30</v>
-          </cell>
-          <cell r="B31">
-            <v>43048</v>
-          </cell>
-          <cell r="C31">
-            <v>42439</v>
-          </cell>
-          <cell r="D31">
-            <v>14879</v>
-          </cell>
-          <cell r="E31">
-            <v>25104</v>
-          </cell>
-        </row>
-        <row r="32">
-          <cell r="A32" t="str">
-            <v>July 31</v>
-          </cell>
-          <cell r="B32">
-            <v>40718</v>
-          </cell>
-          <cell r="C32">
-            <v>34315</v>
-          </cell>
-          <cell r="D32">
-            <v>18579</v>
-          </cell>
-          <cell r="E32">
-            <v>30523</v>
-          </cell>
-        </row>
-        <row r="33">
-          <cell r="A33" t="str">
-            <v>Aug 1</v>
-          </cell>
-          <cell r="B33">
-            <v>24792</v>
-          </cell>
-          <cell r="C33">
-            <v>37711</v>
-          </cell>
-          <cell r="D33">
-            <v>22734</v>
-          </cell>
-          <cell r="E33">
-            <v>30222</v>
-          </cell>
-        </row>
-        <row r="34">
-          <cell r="A34" t="str">
-            <v>Aug 2</v>
-          </cell>
-          <cell r="B34">
-            <v>37548</v>
-          </cell>
-          <cell r="C34">
-            <v>42084</v>
-          </cell>
-          <cell r="D34">
-            <v>17967</v>
-          </cell>
-          <cell r="E34">
-            <v>13064</v>
-          </cell>
-        </row>
-        <row r="35">
-          <cell r="A35" t="str">
-            <v>Aug 3</v>
-          </cell>
-          <cell r="B35">
-            <v>43706</v>
-          </cell>
-          <cell r="C35">
-            <v>55930</v>
-          </cell>
-          <cell r="D35">
-            <v>22848</v>
-          </cell>
-          <cell r="E35">
-            <v>23180</v>
-          </cell>
-        </row>
-        <row r="36">
-          <cell r="A36" t="str">
-            <v>Aug 4</v>
-          </cell>
-          <cell r="B36">
-            <v>41152</v>
-          </cell>
-          <cell r="C36">
-            <v>62687</v>
-          </cell>
-          <cell r="D36">
-            <v>27423</v>
-          </cell>
-          <cell r="E36">
-            <v>20405</v>
-          </cell>
-        </row>
-        <row r="37">
-          <cell r="A37" t="str">
-            <v>Aug 5</v>
-          </cell>
-          <cell r="B37">
-            <v>39293</v>
-          </cell>
-          <cell r="C37">
-            <v>72712</v>
-          </cell>
-          <cell r="D37">
-            <v>31944</v>
-          </cell>
-          <cell r="E37">
-            <v>17137</v>
-          </cell>
-        </row>
-        <row r="38">
-          <cell r="A38" t="str">
-            <v>Aug 6</v>
-          </cell>
-          <cell r="B38">
-            <v>40686</v>
-          </cell>
-          <cell r="C38">
-            <v>76394</v>
-          </cell>
-          <cell r="D38">
-            <v>30190</v>
-          </cell>
-          <cell r="E38">
-            <v>32544</v>
-          </cell>
-        </row>
-        <row r="39">
-          <cell r="A39" t="str">
-            <v>Aug 7</v>
-          </cell>
-          <cell r="B39">
-            <v>26737</v>
-          </cell>
-          <cell r="C39">
-            <v>61264</v>
-          </cell>
-          <cell r="D39">
-            <v>55768</v>
-          </cell>
-          <cell r="E39">
-            <v>56283</v>
-          </cell>
-        </row>
-        <row r="40">
-          <cell r="A40" t="str">
-            <v>Aug 8</v>
-          </cell>
-          <cell r="B40">
-            <v>25520</v>
-          </cell>
-          <cell r="C40">
-            <v>48046</v>
-          </cell>
-          <cell r="D40">
-            <v>11146</v>
-          </cell>
-          <cell r="E40">
-            <v>30678</v>
-          </cell>
-        </row>
-        <row r="41">
-          <cell r="A41" t="str">
-            <v>Aug 9</v>
-          </cell>
-          <cell r="B41">
-            <v>35474</v>
-          </cell>
-          <cell r="C41">
-            <v>37042</v>
-          </cell>
-          <cell r="D41">
-            <v>14372</v>
-          </cell>
-          <cell r="E41">
-            <v>13072</v>
-          </cell>
-        </row>
-        <row r="42">
-          <cell r="A42" t="str">
-            <v>Aug 10</v>
-          </cell>
-          <cell r="B42">
-            <v>24791</v>
-          </cell>
-          <cell r="C42">
-            <v>32759</v>
-          </cell>
-          <cell r="D42">
-            <v>14265</v>
-          </cell>
-          <cell r="E42">
-            <v>8620</v>
-          </cell>
-        </row>
-        <row r="43">
-          <cell r="A43" t="str">
-            <v>Aug 11</v>
-          </cell>
-          <cell r="B43">
-            <v>44123</v>
-          </cell>
-          <cell r="C43">
-            <v>32146</v>
-          </cell>
-          <cell r="D43">
-            <v>26837</v>
-          </cell>
-          <cell r="E43">
-            <v>13168</v>
-          </cell>
-        </row>
-        <row r="44">
-          <cell r="A44" t="str">
-            <v>Aug 12</v>
-          </cell>
-          <cell r="B44">
-            <v>49097</v>
-          </cell>
-          <cell r="C44">
-            <v>25377</v>
-          </cell>
-          <cell r="D44">
-            <v>40040</v>
-          </cell>
-          <cell r="E44">
-            <v>18558</v>
-          </cell>
-        </row>
-        <row r="45">
-          <cell r="A45" t="str">
-            <v>Aug 13</v>
-          </cell>
-          <cell r="B45">
-            <v>65900</v>
-          </cell>
-          <cell r="C45">
-            <v>22158</v>
-          </cell>
-          <cell r="D45">
-            <v>16205</v>
-          </cell>
-          <cell r="E45">
-            <v>30833</v>
-          </cell>
-        </row>
-        <row r="46">
-          <cell r="A46" t="str">
-            <v>Aug 14</v>
-          </cell>
-          <cell r="B46">
-            <v>107241</v>
-          </cell>
-          <cell r="C46">
-            <v>25809</v>
-          </cell>
-          <cell r="D46">
-            <v>6692</v>
-          </cell>
-          <cell r="E46">
-            <v>35256</v>
-          </cell>
-        </row>
-        <row r="47">
-          <cell r="A47" t="str">
-            <v>Aug 15</v>
-          </cell>
-          <cell r="B47">
-            <v>70055</v>
-          </cell>
-          <cell r="C47">
-            <v>24908</v>
-          </cell>
-          <cell r="D47">
-            <v>12195</v>
-          </cell>
-          <cell r="E47">
-            <v>21046</v>
-          </cell>
-        </row>
-        <row r="48">
-          <cell r="A48" t="str">
-            <v>Aug 16</v>
-          </cell>
-          <cell r="B48">
-            <v>112174</v>
-          </cell>
-          <cell r="C48">
-            <v>22220</v>
-          </cell>
-          <cell r="D48">
-            <v>18030</v>
-          </cell>
-          <cell r="E48">
-            <v>16629</v>
-          </cell>
-        </row>
-        <row r="49">
-          <cell r="A49" t="str">
-            <v>Aug 17</v>
-          </cell>
-          <cell r="B49">
-            <v>134874</v>
-          </cell>
-          <cell r="C49">
-            <v>18146</v>
-          </cell>
-          <cell r="D49">
-            <v>23000</v>
-          </cell>
-          <cell r="E49">
-            <v>30362</v>
-          </cell>
-        </row>
-        <row r="50">
-          <cell r="A50" t="str">
-            <v>Aug 18</v>
-          </cell>
-          <cell r="B50">
-            <v>56939</v>
-          </cell>
-          <cell r="C50">
-            <v>16763</v>
-          </cell>
-          <cell r="D50">
-            <v>26642</v>
-          </cell>
-          <cell r="E50">
-            <v>33151</v>
-          </cell>
-        </row>
-        <row r="51">
-          <cell r="A51" t="str">
-            <v>Aug 19</v>
-          </cell>
-          <cell r="B51">
-            <v>15709</v>
-          </cell>
-          <cell r="C51">
-            <v>10131</v>
-          </cell>
-          <cell r="D51">
-            <v>29068</v>
-          </cell>
-          <cell r="E51">
-            <v>32187</v>
-          </cell>
-        </row>
-        <row r="52">
-          <cell r="A52" t="str">
-            <v>Aug 20</v>
-          </cell>
-          <cell r="B52">
-            <v>43468</v>
-          </cell>
-          <cell r="D52">
-            <v>27787</v>
-          </cell>
-          <cell r="E52">
-            <v>23203</v>
-          </cell>
-        </row>
-        <row r="53">
-          <cell r="A53" t="str">
-            <v>Aug 21</v>
-          </cell>
-          <cell r="B53">
-            <v>43826</v>
-          </cell>
-          <cell r="D53">
-            <v>17005</v>
-          </cell>
-          <cell r="E53">
-            <v>20586</v>
-          </cell>
-        </row>
-        <row r="54">
-          <cell r="A54" t="str">
-            <v>Aug 22</v>
-          </cell>
-          <cell r="B54">
-            <v>20828</v>
-          </cell>
-          <cell r="D54">
-            <v>6539</v>
-          </cell>
-          <cell r="E54">
-            <v>12087</v>
-          </cell>
-        </row>
-        <row r="55">
-          <cell r="A55" t="str">
-            <v>Aug 23</v>
-          </cell>
-          <cell r="B55">
-            <v>17402</v>
-          </cell>
-          <cell r="D55">
-            <v>28895</v>
-          </cell>
-          <cell r="E55">
-            <v>12268</v>
-          </cell>
-        </row>
-        <row r="56">
-          <cell r="A56" t="str">
-            <v>Aug 24</v>
-          </cell>
-          <cell r="B56">
-            <v>4785</v>
-          </cell>
-          <cell r="D56">
-            <v>17189</v>
-          </cell>
-          <cell r="E56">
-            <v>16610</v>
-          </cell>
-        </row>
-        <row r="57">
-          <cell r="A57" t="str">
-            <v>Aug 25</v>
-          </cell>
-          <cell r="D57">
-            <v>19651</v>
-          </cell>
-        </row>
-        <row r="58">
-          <cell r="A58" t="str">
-            <v>Aug 26</v>
-          </cell>
-          <cell r="D58">
-            <v>7795</v>
-          </cell>
-        </row>
-        <row r="59">
-          <cell r="A59" t="str">
-            <v>Aug 27</v>
-          </cell>
-          <cell r="D59">
-            <v>9351</v>
-          </cell>
-        </row>
-        <row r="60">
-          <cell r="A60" t="str">
-            <v>Aug 28</v>
-          </cell>
-          <cell r="D60">
-            <v>1436</v>
-          </cell>
+          <cell r="I15"/>
         </row>
       </sheetData>
+      <sheetData sheetId="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -11253,8 +9185,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11501,8 +9433,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E60"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13535,10 +11467,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AI17"/>
+  <dimension ref="A1:AI18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16:K16"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13948,7 +11880,12 @@
       <c r="J16" s="239"/>
       <c r="K16" s="240"/>
     </row>
-    <row r="17" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="17" spans="5:5" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="18" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E18" t="s">
+        <v>220</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="14">
     <mergeCell ref="A15:K15"/>
@@ -14529,8 +12466,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L76"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.3"/>

</xml_diff>